<commit_message>
Fixed imcomplete phrase setup. Had to with leading and trailing spaces
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BBBC6F-7E78-40A5-98D0-64D4CB8875DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514C1B6-CC0C-48D0-AF08-CBD390A9ADAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,51 +124,27 @@
     <t>894499A</t>
   </si>
   <si>
-    <t>Cheese &amp; Spinach 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000026</t>
   </si>
   <si>
-    <t>Cheese Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000019</t>
   </si>
   <si>
-    <t>Goat Cheese Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000156</t>
   </si>
   <si>
-    <t>Lobster Ravioli 48ct, 20oz</t>
-  </si>
-  <si>
     <t>692215800072</t>
   </si>
   <si>
-    <t>Meat &amp; Spinach Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000200</t>
   </si>
   <si>
-    <t>Mushroom Ravioli 48 Ct, 20 oz</t>
-  </si>
-  <si>
     <t>692159000033</t>
   </si>
   <si>
-    <t>Pumpkin Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000255</t>
   </si>
   <si>
-    <t>Roasted Red Pepper Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000040</t>
   </si>
   <si>
@@ -275,6 +251,30 @@
   </si>
   <si>
     <t>Plain Egg Pappardelle</t>
+  </si>
+  <si>
+    <t>Roasted Red Pepper Ravioli</t>
+  </si>
+  <si>
+    <t>Pumpkin Ravioli</t>
+  </si>
+  <si>
+    <t>Mushroom Ravioli</t>
+  </si>
+  <si>
+    <t>Meat &amp; Spinach</t>
+  </si>
+  <si>
+    <t>Lobster Ravioli</t>
+  </si>
+  <si>
+    <t>Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Goat Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Cheese + Spinach</t>
   </si>
 </sst>
 </file>
@@ -556,11 +556,11 @@
   </sheetPr>
   <dimension ref="A1:B1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -572,7 +572,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3">
         <v>692159010100</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3">
         <v>692159010101</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3">
         <v>692159010102</v>
@@ -820,66 +820,66 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -888,18 +888,18 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -908,26 +908,26 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -936,74 +936,74 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1012,18 +1012,18 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2">

</xml_diff>

<commit_message>
Added UI elements. Reworked into one screen and added step counters as well as partial results showing
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514C1B6-CC0C-48D0-AF08-CBD390A9ADAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BBBC6F-7E78-40A5-98D0-64D4CB8875DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,27 +124,51 @@
     <t>894499A</t>
   </si>
   <si>
+    <t>Cheese &amp; Spinach 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000026</t>
   </si>
   <si>
+    <t>Cheese Ravioli 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000019</t>
   </si>
   <si>
+    <t>Goat Cheese Ravioli 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000156</t>
   </si>
   <si>
+    <t>Lobster Ravioli 48ct, 20oz</t>
+  </si>
+  <si>
     <t>692215800072</t>
   </si>
   <si>
+    <t>Meat &amp; Spinach Ravioli 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000200</t>
   </si>
   <si>
+    <t>Mushroom Ravioli 48 Ct, 20 oz</t>
+  </si>
+  <si>
     <t>692159000033</t>
   </si>
   <si>
+    <t>Pumpkin Ravioli 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000255</t>
   </si>
   <si>
+    <t>Roasted Red Pepper Ravioli 48 Ct, 20oz</t>
+  </si>
+  <si>
     <t>692159000040</t>
   </si>
   <si>
@@ -251,30 +275,6 @@
   </si>
   <si>
     <t>Plain Egg Pappardelle</t>
-  </si>
-  <si>
-    <t>Roasted Red Pepper Ravioli</t>
-  </si>
-  <si>
-    <t>Pumpkin Ravioli</t>
-  </si>
-  <si>
-    <t>Mushroom Ravioli</t>
-  </si>
-  <si>
-    <t>Meat &amp; Spinach</t>
-  </si>
-  <si>
-    <t>Lobster Ravioli</t>
-  </si>
-  <si>
-    <t>Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>Goat Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>Cheese + Spinach</t>
   </si>
 </sst>
 </file>
@@ -556,11 +556,11 @@
   </sheetPr>
   <dimension ref="A1:B1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -572,7 +572,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3">
         <v>692159010100</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3">
         <v>692159010101</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3">
         <v>692159010102</v>
@@ -820,66 +820,66 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -888,18 +888,18 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -908,26 +908,26 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -936,74 +936,74 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1012,18 +1012,18 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:2">

</xml_diff>

<commit_message>
Fully working full matching for all matching schema. Need more rigirous testing
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BBBC6F-7E78-40A5-98D0-64D4CB8875DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3450702C-8618-4408-A0FC-742EC82408B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="3825" windowWidth="31935" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>894499A</t>
   </si>
   <si>
-    <t>Cheese &amp; Spinach 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000026</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>692159000019</t>
   </si>
   <si>
-    <t>Goat Cheese Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000156</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
     <t>692159000255</t>
   </si>
   <si>
-    <t>Roasted Red Pepper Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
     <t>692159000040</t>
   </si>
   <si>
@@ -275,6 +266,15 @@
   </si>
   <si>
     <t>Plain Egg Pappardelle</t>
+  </si>
+  <si>
+    <t>Cheese + Spinach Ravioli</t>
+  </si>
+  <si>
+    <t>Goat Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Roasted Red Pepper Ravioli</t>
   </si>
 </sst>
 </file>
@@ -556,11 +556,11 @@
   </sheetPr>
   <dimension ref="A1:B1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -572,7 +572,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3">
         <v>692159010100</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3">
         <v>692159010101</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3">
         <v>692159010102</v>
@@ -820,66 +820,66 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -888,18 +888,18 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -908,26 +908,26 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -936,74 +936,74 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1012,18 +1012,18 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:2">

</xml_diff>

<commit_message>
Changed Configsetup Excel to use local referencing of the UPC codes
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3450702C-8618-4408-A0FC-742EC82408B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F57151-446C-40D9-AC86-9680FC6B6598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="3825" windowWidth="31935" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12060" yWindow="420" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Item Name</t>
   </si>
@@ -181,9 +181,6 @@
     <t>692159005090</t>
   </si>
   <si>
-    <t>Lasagne with Meat</t>
-  </si>
-  <si>
     <t>092159005104</t>
   </si>
   <si>
@@ -275,6 +272,12 @@
   </si>
   <si>
     <t>Roasted Red Pepper Ravioli</t>
+  </si>
+  <si>
+    <t>Meat Lasagna</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -556,8 +559,8 @@
   </sheetPr>
   <dimension ref="A1:B1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -572,7 +575,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3">
         <v>692159010100</v>
@@ -580,7 +583,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3">
         <v>692159010101</v>
@@ -588,7 +591,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3">
         <v>692159010102</v>
@@ -820,7 +823,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>34</v>
@@ -836,7 +839,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>37</v>
@@ -876,7 +879,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>46</v>
@@ -916,18 +919,18 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -936,74 +939,74 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1012,18 +1015,18 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1031,8 +1034,12 @@
       <c r="B63" s="1"/>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="1">
+        <v>123</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1"/>

</xml_diff>

<commit_message>
Updated ConfigSetup to be much cleaner and prevent duplicates. Added at a glance feature to copypastepacker
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F57151-446C-40D9-AC86-9680FC6B6598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ABC041-9218-40A7-B05D-AB2D54A5899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12060" yWindow="420" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:B1021"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added CTRL+M for matching. In progress of adding consistent scroll
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BlueSystem\CopyPastePack\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ABC041-9218-40A7-B05D-AB2D54A5899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1404CC07-4FCE-4487-BF93-9C9A45585B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12060" yWindow="420" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
   <si>
     <t>Item Name</t>
   </si>
@@ -31,253 +31,277 @@
     <t>Spinach Linguine</t>
   </si>
   <si>
+    <t>Spinach Pappardelle</t>
+  </si>
+  <si>
+    <t>Rosemary Linguine</t>
+  </si>
+  <si>
+    <t>Rosemary Fettuccine</t>
+  </si>
+  <si>
+    <t>Rosemary Pappardelle</t>
+  </si>
+  <si>
+    <t>Black Pepper Linguine</t>
+  </si>
+  <si>
+    <t>Black Pepper Fettuccine</t>
+  </si>
+  <si>
+    <t>Black Pepper Pappardelle</t>
+  </si>
+  <si>
+    <t>Lemon Linguine</t>
+  </si>
+  <si>
+    <t>Lemon Fettuccine</t>
+  </si>
+  <si>
+    <t>Lemon Pappardelle</t>
+  </si>
+  <si>
+    <t>Lemon Red Pepper Linguine</t>
+  </si>
+  <si>
+    <t>Lemon Red Pepper Fettuccine</t>
+  </si>
+  <si>
+    <t>Lemon Red Pepper Pappardelle</t>
+  </si>
+  <si>
+    <t>Whole Wheat Linguine</t>
+  </si>
+  <si>
+    <t>Whole Wheat Fettuccine</t>
+  </si>
+  <si>
+    <t>Whole Wheat Pappardelle</t>
+  </si>
+  <si>
+    <t>Squid Ink Linguine</t>
+  </si>
+  <si>
+    <t>Squid Ink Fettuccine</t>
+  </si>
+  <si>
+    <t>Cheese Gnocchi</t>
+  </si>
+  <si>
+    <t>692159005182</t>
+  </si>
+  <si>
+    <t>Potato Gnocchi</t>
+  </si>
+  <si>
+    <t>692159005168</t>
+  </si>
+  <si>
+    <t>Spinach Gnocchi</t>
+  </si>
+  <si>
+    <t>692159005175</t>
+  </si>
+  <si>
+    <t>Jumbo Beet and Goat Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>C579115</t>
+  </si>
+  <si>
+    <t>Jumbo Broccoli Rabe Ravioli</t>
+  </si>
+  <si>
+    <t>P502065</t>
+  </si>
+  <si>
+    <t>894499A</t>
+  </si>
+  <si>
+    <t>692159000026</t>
+  </si>
+  <si>
+    <t>692159000019</t>
+  </si>
+  <si>
+    <t>692159000156</t>
+  </si>
+  <si>
+    <t>692215800072</t>
+  </si>
+  <si>
+    <t>692159000200</t>
+  </si>
+  <si>
+    <t>692159000033</t>
+  </si>
+  <si>
+    <t>692159000255</t>
+  </si>
+  <si>
+    <t>692159000040</t>
+  </si>
+  <si>
+    <t>692159005137</t>
+  </si>
+  <si>
+    <t>Ciliegine Salad</t>
+  </si>
+  <si>
+    <t>692159005328</t>
+  </si>
+  <si>
+    <t>Cheese Lasagne</t>
+  </si>
+  <si>
+    <t>692159005090</t>
+  </si>
+  <si>
+    <t>092159005104</t>
+  </si>
+  <si>
+    <t>Macaroni &amp; Cheese</t>
+  </si>
+  <si>
+    <t>692159006103</t>
+  </si>
+  <si>
+    <t>692159005120</t>
+  </si>
+  <si>
+    <t>692159005076</t>
+  </si>
+  <si>
+    <t>692159005007</t>
+  </si>
+  <si>
+    <t>692159005038</t>
+  </si>
+  <si>
+    <t>692159006073</t>
+  </si>
+  <si>
+    <t>692159005052</t>
+  </si>
+  <si>
+    <t>692159005069</t>
+  </si>
+  <si>
+    <t>692159006080</t>
+  </si>
+  <si>
+    <t>692159005045</t>
+  </si>
+  <si>
+    <t>692159005601</t>
+  </si>
+  <si>
+    <t>692159005618</t>
+  </si>
+  <si>
+    <t>Plain Egg Linguine</t>
+  </si>
+  <si>
+    <t>Plain Egg Fettuccine</t>
+  </si>
+  <si>
+    <t>Plain Egg Pappardelle</t>
+  </si>
+  <si>
+    <t>Cheese + Spinach Ravioli</t>
+  </si>
+  <si>
+    <t>Goat Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Roasted Red Pepper Ravioli</t>
+  </si>
+  <si>
+    <t>Meat Lasagne</t>
+  </si>
+  <si>
+    <t>Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Lobster Ravioli</t>
+  </si>
+  <si>
+    <t>Mushroom Ravioli</t>
+  </si>
+  <si>
+    <t>Pumpkin Ravioli</t>
+  </si>
+  <si>
+    <t>Sauce: Bolognese</t>
+  </si>
+  <si>
+    <t>Sauce: Marinara</t>
+  </si>
+  <si>
+    <t>Sauce: Mushroom Pesto</t>
+  </si>
+  <si>
+    <t>Sauce: Puttanesca</t>
+  </si>
+  <si>
+    <t>Sauce: Sun-dried Tomato Pesto</t>
+  </si>
+  <si>
+    <t>Cheese Tortelloni</t>
+  </si>
+  <si>
+    <t>Pumpkin Tortelloni</t>
+  </si>
+  <si>
+    <t>Sauce: Tomato Basil</t>
+  </si>
+  <si>
+    <t>Sauce: Pink Sauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Cheese + Spinach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Lobster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Mushroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Pumpkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Roasted Red Pepper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Goat Cheese</t>
+  </si>
+  <si>
+    <t>Rice Pudding</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Meat + Spinach</t>
+  </si>
+  <si>
+    <t>Sauce: Pesto</t>
+  </si>
+  <si>
+    <t>Sauce: Arrabiata</t>
+  </si>
+  <si>
     <t>Spinach Fettuccine</t>
   </si>
   <si>
-    <t>Spinach Pappardelle</t>
-  </si>
-  <si>
-    <t>Rosemary Linguine</t>
-  </si>
-  <si>
-    <t>Rosemary Fettuccine</t>
-  </si>
-  <si>
-    <t>Rosemary Pappardelle</t>
-  </si>
-  <si>
-    <t>Black Pepper Linguine</t>
-  </si>
-  <si>
-    <t>Black Pepper Fettuccine</t>
-  </si>
-  <si>
-    <t>Black Pepper Pappardelle</t>
-  </si>
-  <si>
-    <t>Lemon Linguine</t>
-  </si>
-  <si>
-    <t>Lemon Fettuccine</t>
-  </si>
-  <si>
-    <t>Lemon Pappardelle</t>
-  </si>
-  <si>
-    <t>Lemon Red Pepper Linguine</t>
-  </si>
-  <si>
-    <t>Lemon Red Pepper Fettuccine</t>
-  </si>
-  <si>
-    <t>Lemon Red Pepper Pappardelle</t>
-  </si>
-  <si>
-    <t>Whole Wheat Linguine</t>
-  </si>
-  <si>
-    <t>Whole Wheat Fettuccine</t>
-  </si>
-  <si>
-    <t>Whole Wheat Pappardelle</t>
-  </si>
-  <si>
-    <t>Squid Ink Linguine</t>
-  </si>
-  <si>
-    <t>Squid Ink Fettuccine</t>
-  </si>
-  <si>
-    <t>Cheese Gnocchi</t>
-  </si>
-  <si>
-    <t>692159005182</t>
-  </si>
-  <si>
-    <t>Potato Gnocchi</t>
-  </si>
-  <si>
-    <t>692159005168</t>
-  </si>
-  <si>
-    <t>Spinach Gnocchi</t>
-  </si>
-  <si>
-    <t>692159005175</t>
-  </si>
-  <si>
-    <t>Jumbo Beet and Goat Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>C579115</t>
-  </si>
-  <si>
-    <t>Jumbo Broccoli Rabe Ravioli</t>
-  </si>
-  <si>
-    <t>P502065</t>
-  </si>
-  <si>
-    <t>Jumbo Eggplant Pomodoro Ravioli</t>
-  </si>
-  <si>
-    <t>894499A</t>
-  </si>
-  <si>
-    <t>692159000026</t>
-  </si>
-  <si>
-    <t>Cheese Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
-    <t>692159000019</t>
-  </si>
-  <si>
-    <t>692159000156</t>
-  </si>
-  <si>
-    <t>Lobster Ravioli 48ct, 20oz</t>
-  </si>
-  <si>
-    <t>692215800072</t>
-  </si>
-  <si>
-    <t>Meat &amp; Spinach Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
-    <t>692159000200</t>
-  </si>
-  <si>
-    <t>Mushroom Ravioli 48 Ct, 20 oz</t>
-  </si>
-  <si>
-    <t>692159000033</t>
-  </si>
-  <si>
-    <t>Pumpkin Ravioli 48 Ct, 20oz</t>
-  </si>
-  <si>
-    <t>692159000255</t>
-  </si>
-  <si>
-    <t>692159000040</t>
-  </si>
-  <si>
-    <t>Arborio Rice Pudding</t>
-  </si>
-  <si>
-    <t>692159005137</t>
-  </si>
-  <si>
-    <t>Ciliegine Salad</t>
-  </si>
-  <si>
-    <t>692159005328</t>
-  </si>
-  <si>
-    <t>Cheese Lasagne</t>
-  </si>
-  <si>
-    <t>692159005090</t>
-  </si>
-  <si>
-    <t>092159005104</t>
-  </si>
-  <si>
-    <t>Macaroni &amp; Cheese</t>
-  </si>
-  <si>
-    <t>692159006103</t>
-  </si>
-  <si>
-    <t>Arrabbiata Sauce</t>
-  </si>
-  <si>
-    <t>692159005120</t>
-  </si>
-  <si>
-    <t>Bolognese Sauce</t>
-  </si>
-  <si>
-    <t>692159005076</t>
-  </si>
-  <si>
-    <t>Classic Pesto Sauce</t>
-  </si>
-  <si>
-    <t>692159005007</t>
-  </si>
-  <si>
-    <t>Marinara</t>
-  </si>
-  <si>
-    <t>692159005038</t>
-  </si>
-  <si>
-    <t>Mushroom Pesto</t>
-  </si>
-  <si>
-    <t>692159006073</t>
-  </si>
-  <si>
-    <t>Pink Sauce</t>
-  </si>
-  <si>
-    <t>692159005052</t>
-  </si>
-  <si>
-    <t>Puttanesca Sauce</t>
-  </si>
-  <si>
-    <t>692159005069</t>
-  </si>
-  <si>
-    <t>Sun-dried Tomato Pesto</t>
-  </si>
-  <si>
-    <t>692159006080</t>
-  </si>
-  <si>
-    <t>Tomato &amp; Basil Sauce</t>
-  </si>
-  <si>
-    <t>692159005045</t>
-  </si>
-  <si>
-    <t>Cheese Tortelloni 16oz.</t>
-  </si>
-  <si>
-    <t>692159005601</t>
-  </si>
-  <si>
-    <t>Pumpkin Tortelloni 16oz.</t>
-  </si>
-  <si>
-    <t>692159005618</t>
-  </si>
-  <si>
-    <t>Plain Egg Linguine</t>
-  </si>
-  <si>
-    <t>Plain Egg Fettuccine</t>
-  </si>
-  <si>
-    <t>Plain Egg Pappardelle</t>
-  </si>
-  <si>
-    <t>Cheese + Spinach Ravioli</t>
-  </si>
-  <si>
-    <t>Goat Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>Roasted Red Pepper Ravioli</t>
-  </si>
-  <si>
-    <t>Meat Lasagna</t>
-  </si>
-  <si>
-    <t>asdf</t>
+    <t>Jumbo Eggplant Ravioli</t>
+  </si>
+  <si>
+    <t>Sauce: Sage Butter</t>
+  </si>
+  <si>
+    <t>Meat + Spinach Ravioli</t>
   </si>
 </sst>
 </file>
@@ -557,10 +581,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1021"/>
+  <dimension ref="A1:B1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -575,7 +599,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3">
         <v>692159010100</v>
@@ -583,7 +607,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3">
         <v>692159010101</v>
@@ -591,7 +615,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3">
         <v>692159010102</v>
@@ -607,7 +631,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3">
         <v>692159010104</v>
@@ -615,7 +639,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
         <v>692159010105</v>
@@ -623,7 +647,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>692159010106</v>
@@ -631,7 +655,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>692159010107</v>
@@ -639,7 +663,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>692159010108</v>
@@ -647,7 +671,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3">
         <v>692159010109</v>
@@ -655,7 +679,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3">
         <v>692159010110</v>
@@ -663,7 +687,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3">
         <v>692159010111</v>
@@ -671,7 +695,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>692159010112</v>
@@ -679,7 +703,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>692159010113</v>
@@ -687,7 +711,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3">
         <v>692159010114</v>
@@ -695,7 +719,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3">
         <v>692159010115</v>
@@ -703,7 +727,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="3">
         <v>692159010116</v>
@@ -711,7 +735,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3">
         <v>692159010117</v>
@@ -719,7 +743,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3">
         <v>692159010118</v>
@@ -727,7 +751,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3">
         <v>692159010119</v>
@@ -735,7 +759,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <v>692159010120</v>
@@ -743,7 +767,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3">
         <v>692159010121</v>
@@ -751,7 +775,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
         <v>692159010122</v>
@@ -767,26 +791,26 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -795,26 +819,26 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -823,66 +847,66 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -891,18 +915,18 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -911,26 +935,26 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -939,139 +963,171 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="1"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="5">
+        <v>111</v>
+      </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
+      <c r="B63" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="B67" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="A68" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+      <c r="A70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="A72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1"/>
@@ -4868,6 +4924,10 @@
     <row r="1021" spans="1:2">
       <c r="A1021" s="1"/>
       <c r="B1021" s="1"/>
+    </row>
+    <row r="1022" spans="1:2">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added product images folder. Works with an image.
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BlueSystem\CopyPastePack\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1404CC07-4FCE-4487-BF93-9C9A45585B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F910E56C-E5B7-443B-A710-2CEA8F37A1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="420" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Item Name</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>Meat + Spinach Ravioli</t>
+  </si>
+  <si>
+    <t>./product_images/MacAndCheese.jpg</t>
   </si>
 </sst>
 </file>
@@ -581,10 +584,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1022"/>
+  <dimension ref="A1:C1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -949,19 +952,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1"/>
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
         <v>89</v>
       </c>
@@ -969,7 +975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
         <v>70</v>
       </c>
@@ -977,7 +983,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>88</v>
       </c>
@@ -985,7 +991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
@@ -993,7 +999,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
         <v>72</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
         <v>78</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
         <v>73</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
         <v>74</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
         <v>77</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
         <v>92</v>
       </c>
@@ -1041,11 +1047,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61" s="1"/>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>75</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>76</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
     </row>

</xml_diff>

<commit_message>
Partially working. Changes needed for special character replacement between both programs
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F910E56C-E5B7-443B-A710-2CEA8F37A1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BE3935-37D5-475F-B418-B1F11994DEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,8 +586,8 @@
   </sheetPr>
   <dimension ref="A1:C1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
CHanged UPC codes to cut off and only match on 11 digits as the last digit is a check digit and is uneeded and weird
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BE3935-37D5-475F-B418-B1F11994DEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t>Item Name</t>
   </si>
@@ -88,9 +82,6 @@
     <t>Cheese Gnocchi</t>
   </si>
   <si>
-    <t>692159005182</t>
-  </si>
-  <si>
     <t>Potato Gnocchi</t>
   </si>
   <si>
@@ -106,18 +97,9 @@
     <t>Jumbo Beet and Goat Cheese Ravioli</t>
   </si>
   <si>
-    <t>C579115</t>
-  </si>
-  <si>
     <t>Jumbo Broccoli Rabe Ravioli</t>
   </si>
   <si>
-    <t>P502065</t>
-  </si>
-  <si>
-    <t>894499A</t>
-  </si>
-  <si>
     <t>692159000026</t>
   </si>
   <si>
@@ -157,9 +139,6 @@
     <t>692159005090</t>
   </si>
   <si>
-    <t>092159005104</t>
-  </si>
-  <si>
     <t>Macaroni &amp; Cheese</t>
   </si>
   <si>
@@ -305,12 +284,18 @@
   </si>
   <si>
     <t>./product_images/MacAndCheese.jpg</t>
+  </si>
+  <si>
+    <t>Truffle Ravioli</t>
+  </si>
+  <si>
+    <t>Ravioli: Truffle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -580,17 +565,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1022"/>
+  <dimension ref="A1:C1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -602,26 +590,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3">
-        <v>692159010100</v>
+        <v>69215901001</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3">
-        <v>692159010101</v>
+        <v>69215901002</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3">
-        <v>692159010102</v>
+        <v>69215901003</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -629,15 +617,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>692159010103</v>
+        <v>69215901004</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3">
-        <v>692159010104</v>
+        <v>69215901005</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -645,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>692159010105</v>
+        <v>69215901006</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -653,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>692159010106</v>
+        <v>69215901007</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -661,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>692159010107</v>
+        <v>69215901008</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -669,7 +657,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>692159010108</v>
+        <v>69215901009</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -677,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>692159010109</v>
+        <v>69215901010</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -685,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>692159010110</v>
+        <v>69215901011</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -693,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>692159010111</v>
+        <v>69215901012</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -701,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>692159010112</v>
+        <v>69215901013</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -709,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3">
-        <v>692159010113</v>
+        <v>69215901014</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -717,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3">
-        <v>692159010114</v>
+        <v>69215901015</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -725,7 +713,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="3">
-        <v>692159010115</v>
+        <v>69215901016</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -733,7 +721,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="3">
-        <v>692159010116</v>
+        <v>69215901017</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -741,7 +729,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <v>692159010117</v>
+        <v>69215901018</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -749,7 +737,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>692159010118</v>
+        <v>69215901019</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -757,7 +745,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="3">
-        <v>692159010119</v>
+        <v>69215901020</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -765,7 +753,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="3">
-        <v>692159010120</v>
+        <v>69215901021</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -773,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3">
-        <v>692159010121</v>
+        <v>69215901022</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -781,7 +769,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="3">
-        <v>692159010122</v>
+        <v>69215901023</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -796,24 +784,24 @@
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>22</v>
+      <c r="B27" s="5">
+        <v>692159005182</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -822,26 +810,26 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B31" s="5">
+        <v>692159000422</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="5">
+        <v>692159000439</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>86</v>
+      </c>
+      <c r="B33" s="5">
+        <v>692159000415</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -850,169 +838,167 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
+      </c>
+      <c r="B35" s="5">
+        <v>692159000026</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="B36" s="5">
+        <v>692159000019</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>36</v>
+        <v>88</v>
+      </c>
+      <c r="B39" s="5">
+        <v>692159000200</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>94</v>
+        <v>60</v>
+      </c>
+      <c r="B49" s="5">
+        <v>692159005104</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1020,95 +1006,95 @@
         <v>73</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="5">
+        <v>72</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="5">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="4"/>
-    </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="A64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1116,31 +1102,37 @@
         <v>82</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B74" s="1"/>
     </row>
     <row r="75" spans="1:2">
@@ -4934,6 +4926,10 @@
     <row r="1022" spans="1:2">
       <c r="A1022" s="1"/>
       <c r="B1022" s="1"/>
+    </row>
+    <row r="1023" spans="1:2">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed barcodes to strings to preserve leading 0's
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B3EBD-63D7-4828-BC43-1BDF9156B5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>Item Name</t>
   </si>
@@ -136,166 +142,172 @@
     <t>Cheese Lasagne</t>
   </si>
   <si>
+    <t>Macaroni &amp; Cheese</t>
+  </si>
+  <si>
+    <t>692159006103</t>
+  </si>
+  <si>
+    <t>692159005120</t>
+  </si>
+  <si>
+    <t>692159005076</t>
+  </si>
+  <si>
+    <t>692159005007</t>
+  </si>
+  <si>
+    <t>692159005038</t>
+  </si>
+  <si>
+    <t>692159006073</t>
+  </si>
+  <si>
+    <t>692159005052</t>
+  </si>
+  <si>
+    <t>692159005069</t>
+  </si>
+  <si>
+    <t>692159006080</t>
+  </si>
+  <si>
+    <t>692159005045</t>
+  </si>
+  <si>
+    <t>692159005601</t>
+  </si>
+  <si>
+    <t>692159005618</t>
+  </si>
+  <si>
+    <t>Plain Egg Linguine</t>
+  </si>
+  <si>
+    <t>Plain Egg Fettuccine</t>
+  </si>
+  <si>
+    <t>Plain Egg Pappardelle</t>
+  </si>
+  <si>
+    <t>Cheese + Spinach Ravioli</t>
+  </si>
+  <si>
+    <t>Goat Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Roasted Red Pepper Ravioli</t>
+  </si>
+  <si>
+    <t>Meat Lasagne</t>
+  </si>
+  <si>
+    <t>Cheese Ravioli</t>
+  </si>
+  <si>
+    <t>Lobster Ravioli</t>
+  </si>
+  <si>
+    <t>Mushroom Ravioli</t>
+  </si>
+  <si>
+    <t>Pumpkin Ravioli</t>
+  </si>
+  <si>
+    <t>Sauce: Bolognese</t>
+  </si>
+  <si>
+    <t>Sauce: Marinara</t>
+  </si>
+  <si>
+    <t>Sauce: Mushroom Pesto</t>
+  </si>
+  <si>
+    <t>Sauce: Puttanesca</t>
+  </si>
+  <si>
+    <t>Sauce: Sun-dried Tomato Pesto</t>
+  </si>
+  <si>
+    <t>Cheese Tortelloni</t>
+  </si>
+  <si>
+    <t>Pumpkin Tortelloni</t>
+  </si>
+  <si>
+    <t>Sauce: Tomato Basil</t>
+  </si>
+  <si>
+    <t>Sauce: Pink Sauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Cheese + Spinach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Lobster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Mushroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Pumpkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Roasted Red Pepper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Goat Cheese</t>
+  </si>
+  <si>
+    <t>Rice Pudding</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravioli: Meat + Spinach</t>
+  </si>
+  <si>
+    <t>Sauce: Pesto</t>
+  </si>
+  <si>
+    <t>Sauce: Arrabiata</t>
+  </si>
+  <si>
+    <t>Spinach Fettuccine</t>
+  </si>
+  <si>
+    <t>Jumbo Eggplant Ravioli</t>
+  </si>
+  <si>
+    <t>Sauce: Sage Butter</t>
+  </si>
+  <si>
+    <t>Meat + Spinach Ravioli</t>
+  </si>
+  <si>
+    <t>./product_images/MacAndCheese.jpg</t>
+  </si>
+  <si>
+    <t>Truffle Ravioli</t>
+  </si>
+  <si>
+    <t>Ravioli: Truffle</t>
+  </si>
+  <si>
+    <t>092159004091</t>
+  </si>
+  <si>
+    <t>092159005104</t>
+  </si>
+  <si>
     <t>692159005090</t>
-  </si>
-  <si>
-    <t>Macaroni &amp; Cheese</t>
-  </si>
-  <si>
-    <t>692159006103</t>
-  </si>
-  <si>
-    <t>692159005120</t>
-  </si>
-  <si>
-    <t>692159005076</t>
-  </si>
-  <si>
-    <t>692159005007</t>
-  </si>
-  <si>
-    <t>692159005038</t>
-  </si>
-  <si>
-    <t>692159006073</t>
-  </si>
-  <si>
-    <t>692159005052</t>
-  </si>
-  <si>
-    <t>692159005069</t>
-  </si>
-  <si>
-    <t>692159006080</t>
-  </si>
-  <si>
-    <t>692159005045</t>
-  </si>
-  <si>
-    <t>692159005601</t>
-  </si>
-  <si>
-    <t>692159005618</t>
-  </si>
-  <si>
-    <t>Plain Egg Linguine</t>
-  </si>
-  <si>
-    <t>Plain Egg Fettuccine</t>
-  </si>
-  <si>
-    <t>Plain Egg Pappardelle</t>
-  </si>
-  <si>
-    <t>Cheese + Spinach Ravioli</t>
-  </si>
-  <si>
-    <t>Goat Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>Roasted Red Pepper Ravioli</t>
-  </si>
-  <si>
-    <t>Meat Lasagne</t>
-  </si>
-  <si>
-    <t>Cheese Ravioli</t>
-  </si>
-  <si>
-    <t>Lobster Ravioli</t>
-  </si>
-  <si>
-    <t>Mushroom Ravioli</t>
-  </si>
-  <si>
-    <t>Pumpkin Ravioli</t>
-  </si>
-  <si>
-    <t>Sauce: Bolognese</t>
-  </si>
-  <si>
-    <t>Sauce: Marinara</t>
-  </si>
-  <si>
-    <t>Sauce: Mushroom Pesto</t>
-  </si>
-  <si>
-    <t>Sauce: Puttanesca</t>
-  </si>
-  <si>
-    <t>Sauce: Sun-dried Tomato Pesto</t>
-  </si>
-  <si>
-    <t>Cheese Tortelloni</t>
-  </si>
-  <si>
-    <t>Pumpkin Tortelloni</t>
-  </si>
-  <si>
-    <t>Sauce: Tomato Basil</t>
-  </si>
-  <si>
-    <t>Sauce: Pink Sauce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Cheese + Spinach</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Cheese</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Lobster</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Mushroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Pumpkin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Roasted Red Pepper</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Goat Cheese</t>
-  </si>
-  <si>
-    <t>Rice Pudding</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ravioli: Meat + Spinach</t>
-  </si>
-  <si>
-    <t>Sauce: Pesto</t>
-  </si>
-  <si>
-    <t>Sauce: Arrabiata</t>
-  </si>
-  <si>
-    <t>Spinach Fettuccine</t>
-  </si>
-  <si>
-    <t>Jumbo Eggplant Ravioli</t>
-  </si>
-  <si>
-    <t>Sauce: Sage Butter</t>
-  </si>
-  <si>
-    <t>Meat + Spinach Ravioli</t>
-  </si>
-  <si>
-    <t>./product_images/MacAndCheese.jpg</t>
-  </si>
-  <si>
-    <t>Truffle Ravioli</t>
-  </si>
-  <si>
-    <t>Ravioli: Truffle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -342,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,6 +363,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,14 +578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -590,7 +603,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3">
         <v>69215901001</v>
@@ -598,7 +611,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3">
         <v>69215901002</v>
@@ -606,7 +619,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3">
         <v>69215901003</v>
@@ -622,7 +635,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3">
         <v>69215901005</v>
@@ -826,7 +839,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="5">
         <v>692159000415</v>
@@ -838,7 +851,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="5">
         <v>692159000026</v>
@@ -846,7 +859,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5">
         <v>692159000019</v>
@@ -854,7 +867,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>30</v>
@@ -862,7 +875,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>31</v>
@@ -870,7 +883,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="5">
         <v>692159000200</v>
@@ -878,7 +891,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>33</v>
@@ -886,7 +899,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>34</v>
@@ -894,7 +907,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>35</v>
@@ -902,7 +915,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="5"/>
     </row>
@@ -912,7 +925,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>36</v>
@@ -934,27 +947,27 @@
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>40</v>
+      <c r="B48" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="5">
-        <v>692159005104</v>
+        <v>59</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -963,82 +976,82 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" s="5">
-        <v>111</v>
+        <v>86</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1047,18 +1060,18 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1067,7 +1080,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>28</v>
@@ -1075,7 +1088,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>29</v>
@@ -1083,7 +1096,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>30</v>
@@ -1091,7 +1104,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>31</v>
@@ -1099,7 +1112,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>32</v>
@@ -1107,7 +1120,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>33</v>
@@ -1115,7 +1128,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>34</v>
@@ -1123,7 +1136,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>35</v>
@@ -1131,7 +1144,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B74" s="1"/>
     </row>
@@ -4933,5 +4946,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added labels to excel items, and added proper error code handling
</commit_message>
<xml_diff>
--- a/CopyPastePackSrc/UPCCodes.xlsx
+++ b/CopyPastePackSrc/UPCCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\CopyPastePackSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B3EBD-63D7-4828-BC43-1BDF9156B5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D3B30-AEDA-45EE-BB98-F9558B5599C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Item Name</t>
   </si>
@@ -302,6 +302,30 @@
   </si>
   <si>
     <t>692159005090</t>
+  </si>
+  <si>
+    <t>Pasta Cuts</t>
+  </si>
+  <si>
+    <t>Gnocchi</t>
+  </si>
+  <si>
+    <t>Speciality Ravioli</t>
+  </si>
+  <si>
+    <t>Ravioli</t>
+  </si>
+  <si>
+    <t>Add Ons</t>
+  </si>
+  <si>
+    <t>Prepared Meals</t>
+  </si>
+  <si>
+    <t>Sauces</t>
+  </si>
+  <si>
+    <t>Tortelloni</t>
   </si>
 </sst>
 </file>
@@ -582,10 +606,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1023"/>
+  <dimension ref="A1:C1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -602,575 +626,595 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="3">
-        <v>69215901001</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3">
-        <v>69215901002</v>
+        <v>69215901001</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3">
-        <v>69215901003</v>
+        <v>69215901002</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3">
-        <v>69215901004</v>
+        <v>69215901003</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>69215901005</v>
+        <v>69215901004</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3">
-        <v>69215901006</v>
+        <v>69215901005</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3">
-        <v>69215901007</v>
+        <v>69215901006</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>69215901008</v>
+        <v>69215901007</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3">
-        <v>69215901009</v>
+        <v>69215901008</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>69215901010</v>
+        <v>69215901009</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>69215901011</v>
+        <v>69215901010</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3">
-        <v>69215901012</v>
+        <v>69215901011</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
-        <v>69215901013</v>
+        <v>69215901012</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
-        <v>69215901014</v>
+        <v>69215901013</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>69215901015</v>
+        <v>69215901014</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
-        <v>69215901016</v>
+        <v>69215901015</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
-        <v>69215901017</v>
+        <v>69215901016</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
-        <v>69215901018</v>
+        <v>69215901017</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
-        <v>69215901019</v>
+        <v>69215901018</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
-        <v>69215901020</v>
+        <v>69215901019</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3">
-        <v>69215901021</v>
+        <v>69215901020</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
-        <v>69215901022</v>
+        <v>69215901021</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3">
+        <v>69215901022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B25" s="3">
         <v>69215901023</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="5">
-        <v>692159005182</v>
-      </c>
+      <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="B28" s="5">
+        <v>692159005182</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="4"/>
-    </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="5">
-        <v>692159000422</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="5">
-        <v>692159000439</v>
-      </c>
+      <c r="A32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="B33" s="5">
-        <v>692159000415</v>
+        <v>692159000422</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="5">
+        <v>692159000439</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B35" s="5">
-        <v>692159000026</v>
+        <v>692159000415</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="5">
-        <v>692159000019</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>31</v>
+        <v>56</v>
+      </c>
+      <c r="B38" s="5">
+        <v>692159000026</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B39" s="5">
-        <v>692159000200</v>
+        <v>692159000019</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="B42" s="5">
+        <v>692159000200</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>38</v>
+        <v>89</v>
+      </c>
+      <c r="B46" s="5">
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>92</v>
+        <v>79</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>45</v>
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="1">
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="A57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="A61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="C64" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B74" s="1"/>
+      <c r="A74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
+      <c r="A75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
+      <c r="A80" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1"/>
@@ -4943,6 +4987,34 @@
     <row r="1023" spans="1:2">
       <c r="A1023" s="1"/>
       <c r="B1023" s="1"/>
+    </row>
+    <row r="1024" spans="1:2">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+    </row>
+    <row r="1025" spans="1:2">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+    </row>
+    <row r="1026" spans="1:2">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+    </row>
+    <row r="1027" spans="1:2">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="1"/>
+    </row>
+    <row r="1028" spans="1:2">
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="1"/>
+    </row>
+    <row r="1029" spans="1:2">
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="1"/>
+    </row>
+    <row r="1030" spans="1:2">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>